<commit_message>
Customer syncs and new CA policies
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen-Basic-ADSync.xlsx
+++ b/data/aad/Gruppen-Basic-ADSync.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5825AC9-6D50-4018-9B68-CA7365D31A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38025EA3-AE86-4AD8-924B-0FE764F8B72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="1680" windowWidth="26916" windowHeight="14316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="30804" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gruppen!$A$1:$T$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gruppen!$A$1:$T$147</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="282">
   <si>
     <t>Type</t>
   </si>
@@ -868,6 +868,12 @@
   </si>
   <si>
     <t>Disables several things for service accounts (MFA, password reset, …)</t>
+  </si>
+  <si>
+    <t>ALYASG-ADM-LEGACYAUTHENABLED</t>
+  </si>
+  <si>
+    <t>Legacy Auth is not blocked by conditional Access for members in this group</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1271,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T146"/>
+  <dimension ref="A1:T147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -1602,13 +1608,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>280</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>280</v>
       </c>
       <c r="E13" t="s">
-        <v>148</v>
+        <v>281</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="s">
@@ -1618,19 +1624,19 @@
     </row>
     <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="s">
@@ -1646,10 +1652,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>196</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>149</v>
       </c>
       <c r="E15" t="s">
         <v>150</v>
@@ -1658,22 +1664,20 @@
       <c r="G15" t="s">
         <v>8</v>
       </c>
-      <c r="R15" t="s">
-        <v>149</v>
-      </c>
+      <c r="R15"/>
     </row>
     <row r="16" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E16" t="s">
         <v>150</v>
@@ -1686,74 +1690,51 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>190</v>
       </c>
       <c r="C17" t="s">
-        <v>278</v>
+        <v>195</v>
       </c>
       <c r="D17" t="s">
-        <v>278</v>
+        <v>195</v>
       </c>
       <c r="E17" t="s">
-        <v>279</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="F17"/>
       <c r="G17" t="s">
         <v>8</v>
       </c>
       <c r="R17" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>167</v>
+        <v>278</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>278</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" t="s">
-        <v>167</v>
+        <v>279</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
       </c>
-      <c r="H18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J18" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" t="b">
-        <v>1</v>
-      </c>
-      <c r="L18" t="b">
-        <v>1</v>
-      </c>
-      <c r="M18" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18" t="b">
-        <v>0</v>
-      </c>
-      <c r="O18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P18" t="b">
-        <v>1</v>
+      <c r="R18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
@@ -1764,22 +1745,22 @@
         <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="J19" t="b">
         <v>1</v>
@@ -1805,28 +1786,28 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>169</v>
       </c>
       <c r="C20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E20" t="s">
-        <v>174</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>170</v>
+        <v>11</v>
       </c>
       <c r="J20" t="b">
         <v>1</v>
@@ -1849,34 +1830,58 @@
       <c r="P20" t="b">
         <v>1</v>
       </c>
-      <c r="S20" t="s">
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" t="b">
+        <v>0</v>
+      </c>
+      <c r="P21" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21" t="s">
         <v>171</v>
       </c>
-      <c r="T20" s="5" t="s">
+      <c r="T21" s="5" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q21" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1887,10 +1892,10 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>198</v>
+        <v>94</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>198</v>
+        <v>94</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>175</v>
@@ -1907,13 +1912,13 @@
         <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>175</v>
@@ -1921,28 +1926,28 @@
       <c r="G23" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="Q23" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>12</v>
+        <v>190</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1953,19 +1958,19 @@
         <v>12</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>186</v>
+        <v>95</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>186</v>
+        <v>95</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>178</v>
+        <v>25</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1976,19 +1981,19 @@
         <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1999,19 +2004,19 @@
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>96</v>
+        <v>187</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>96</v>
+        <v>187</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>28</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2022,19 +2027,19 @@
         <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2045,19 +2050,19 @@
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2068,19 +2073,19 @@
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2091,19 +2096,19 @@
         <v>12</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2114,19 +2119,19 @@
         <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2137,19 +2142,19 @@
         <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2160,19 +2165,19 @@
         <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2183,19 +2188,19 @@
         <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2206,19 +2211,19 @@
         <v>12</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2229,19 +2234,19 @@
         <v>12</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2252,19 +2257,19 @@
         <v>12</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2275,19 +2280,19 @@
         <v>12</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2298,19 +2303,19 @@
         <v>12</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2321,19 +2326,19 @@
         <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2344,19 +2349,19 @@
         <v>12</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2367,19 +2372,19 @@
         <v>12</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2390,19 +2395,19 @@
         <v>12</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2413,19 +2418,19 @@
         <v>12</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2436,19 +2441,19 @@
         <v>12</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2459,19 +2464,19 @@
         <v>12</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2482,19 +2487,19 @@
         <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2505,19 +2510,19 @@
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2528,19 +2533,19 @@
         <v>12</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2551,19 +2556,19 @@
         <v>12</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2574,19 +2579,19 @@
         <v>12</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2597,19 +2602,19 @@
         <v>12</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>276</v>
+        <v>165</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>276</v>
+        <v>165</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>272</v>
+        <v>157</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>273</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2620,39 +2625,42 @@
         <v>12</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H54" s="2" t="s">
+      <c r="G55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2663,10 +2671,10 @@
         <v>12</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>31</v>
@@ -2683,10 +2691,10 @@
         <v>12</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>31</v>
@@ -2703,10 +2711,10 @@
         <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>202</v>
+        <v>117</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>202</v>
+        <v>117</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>31</v>
@@ -2723,10 +2731,10 @@
         <v>12</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>31</v>
@@ -2743,10 +2751,10 @@
         <v>12</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>118</v>
+        <v>199</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>118</v>
+        <v>199</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>31</v>
@@ -2763,19 +2771,16 @@
         <v>12</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="R61" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2786,16 +2791,19 @@
         <v>12</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="R62" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2806,10 +2814,10 @@
         <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>31</v>
@@ -2826,10 +2834,10 @@
         <v>12</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>31</v>
@@ -2846,10 +2854,10 @@
         <v>12</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>31</v>
@@ -2866,10 +2874,10 @@
         <v>12</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>31</v>
@@ -2886,10 +2894,10 @@
         <v>12</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>31</v>
@@ -2906,19 +2914,16 @@
         <v>12</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="R68" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2929,10 +2934,10 @@
         <v>12</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>31</v>
@@ -2952,10 +2957,10 @@
         <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>31</v>
@@ -2975,16 +2980,19 @@
         <v>12</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="R71" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2995,10 +3003,10 @@
         <v>12</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>31</v>
@@ -3015,10 +3023,10 @@
         <v>12</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>31</v>
@@ -3035,10 +3043,10 @@
         <v>12</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>31</v>
@@ -3055,10 +3063,10 @@
         <v>12</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>31</v>
@@ -3075,10 +3083,10 @@
         <v>12</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>31</v>
@@ -3095,10 +3103,10 @@
         <v>12</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>31</v>
@@ -3115,10 +3123,10 @@
         <v>12</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>31</v>
@@ -3135,10 +3143,10 @@
         <v>12</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>262</v>
+        <v>135</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>262</v>
+        <v>135</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>31</v>
@@ -3155,10 +3163,10 @@
         <v>12</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>31</v>
@@ -3175,10 +3183,10 @@
         <v>12</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>31</v>
@@ -3195,7 +3203,7 @@
         <v>12</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>203</v>
@@ -3207,30 +3215,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I83" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="R83" s="6" t="s">
-        <v>116</v>
+    <row r="83" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3241,10 +3243,10 @@
         <v>190</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>31</v>
@@ -3253,10 +3255,10 @@
         <v>8</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="R84" s="6" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3267,10 +3269,10 @@
         <v>190</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>31</v>
@@ -3279,10 +3281,10 @@
         <v>8</v>
       </c>
       <c r="I85" s="6" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="R85" s="6" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3293,10 +3295,10 @@
         <v>190</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>31</v>
@@ -3305,10 +3307,10 @@
         <v>8</v>
       </c>
       <c r="I86" s="6" t="s">
-        <v>201</v>
+        <v>82</v>
       </c>
       <c r="R86" s="6" t="s">
-        <v>202</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3319,10 +3321,10 @@
         <v>190</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>31</v>
@@ -3331,10 +3333,10 @@
         <v>8</v>
       </c>
       <c r="I87" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="R87" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="88" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3345,10 +3347,10 @@
         <v>190</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>31</v>
@@ -3357,10 +3359,10 @@
         <v>8</v>
       </c>
       <c r="I88" s="6" t="s">
-        <v>83</v>
+        <v>200</v>
       </c>
       <c r="R88" s="6" t="s">
-        <v>118</v>
+        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3371,10 +3373,10 @@
         <v>190</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>31</v>
@@ -3383,10 +3385,10 @@
         <v>8</v>
       </c>
       <c r="I89" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R89" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="90" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3397,10 +3399,10 @@
         <v>190</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>31</v>
@@ -3409,10 +3411,10 @@
         <v>8</v>
       </c>
       <c r="I90" s="6" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="R90" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3423,10 +3425,10 @@
         <v>190</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>31</v>
@@ -3435,10 +3437,10 @@
         <v>8</v>
       </c>
       <c r="I91" s="6" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="R91" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3449,10 +3451,10 @@
         <v>190</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>31</v>
@@ -3461,10 +3463,10 @@
         <v>8</v>
       </c>
       <c r="I92" s="6" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="R92" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3475,10 +3477,10 @@
         <v>190</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>31</v>
@@ -3487,10 +3489,10 @@
         <v>8</v>
       </c>
       <c r="I93" s="6" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="R93" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3501,10 +3503,10 @@
         <v>190</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>31</v>
@@ -3513,10 +3515,10 @@
         <v>8</v>
       </c>
       <c r="I94" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R94" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="95" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3527,10 +3529,10 @@
         <v>190</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>31</v>
@@ -3539,10 +3541,10 @@
         <v>8</v>
       </c>
       <c r="I95" s="6" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="R95" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3553,10 +3555,10 @@
         <v>190</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E96" s="6" t="s">
         <v>31</v>
@@ -3565,10 +3567,10 @@
         <v>8</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>145</v>
+        <v>42</v>
       </c>
       <c r="R96" s="6" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3579,10 +3581,10 @@
         <v>190</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>31</v>
@@ -3591,10 +3593,10 @@
         <v>8</v>
       </c>
       <c r="I97" s="6" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="R97" s="6" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3605,10 +3607,10 @@
         <v>190</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>31</v>
@@ -3617,10 +3619,10 @@
         <v>8</v>
       </c>
       <c r="I98" s="6" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="R98" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="99" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3631,10 +3633,10 @@
         <v>190</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>31</v>
@@ -3643,10 +3645,10 @@
         <v>8</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="R99" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="100" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3657,10 +3659,10 @@
         <v>190</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>31</v>
@@ -3669,10 +3671,10 @@
         <v>8</v>
       </c>
       <c r="I100" s="6" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="R100" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="101" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3683,10 +3685,10 @@
         <v>190</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>31</v>
@@ -3695,10 +3697,10 @@
         <v>8</v>
       </c>
       <c r="I101" s="6" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="R101" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="102" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3709,10 +3711,10 @@
         <v>190</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>31</v>
@@ -3721,10 +3723,10 @@
         <v>8</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="R102" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="103" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3735,10 +3737,10 @@
         <v>190</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>31</v>
@@ -3747,10 +3749,10 @@
         <v>8</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="R103" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="104" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3761,10 +3763,10 @@
         <v>190</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>31</v>
@@ -3773,10 +3775,10 @@
         <v>8</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R104" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="105" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3787,10 +3789,10 @@
         <v>190</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>31</v>
@@ -3799,10 +3801,10 @@
         <v>8</v>
       </c>
       <c r="I105" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R105" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="106" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3813,10 +3815,10 @@
         <v>190</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>31</v>
@@ -3825,10 +3827,10 @@
         <v>8</v>
       </c>
       <c r="I106" s="6" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="R106" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="107" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3839,10 +3841,10 @@
         <v>190</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="E107" s="6" t="s">
         <v>31</v>
@@ -3851,10 +3853,10 @@
         <v>8</v>
       </c>
       <c r="I107" s="6" t="s">
-        <v>261</v>
+        <v>44</v>
       </c>
       <c r="R107" s="6" t="s">
-        <v>262</v>
+        <v>135</v>
       </c>
     </row>
     <row r="108" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3865,10 +3867,10 @@
         <v>190</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>31</v>
@@ -3877,10 +3879,10 @@
         <v>8</v>
       </c>
       <c r="I108" s="6" t="s">
-        <v>93</v>
+        <v>261</v>
       </c>
       <c r="R108" s="6" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3891,10 +3893,10 @@
         <v>190</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>31</v>
@@ -3903,10 +3905,10 @@
         <v>8</v>
       </c>
       <c r="I109" s="6" t="s">
-        <v>204</v>
+        <v>93</v>
       </c>
       <c r="R109" s="6" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3917,7 +3919,7 @@
         <v>190</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>270</v>
+        <v>230</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>230</v>
@@ -3929,36 +3931,36 @@
         <v>8</v>
       </c>
       <c r="I110" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="R110" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I111" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="R110" s="6" t="s">
+      <c r="R111" s="6" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I111" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="R111" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3969,10 +3971,10 @@
         <v>12</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>31</v>
@@ -3981,10 +3983,10 @@
         <v>8</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="R112" s="3" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3995,10 +3997,10 @@
         <v>12</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>31</v>
@@ -4007,10 +4009,10 @@
         <v>8</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="R113" s="3" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
     </row>
     <row r="114" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4021,10 +4023,10 @@
         <v>12</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>31</v>
@@ -4033,10 +4035,10 @@
         <v>8</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>201</v>
+        <v>82</v>
       </c>
       <c r="R114" s="3" t="s">
-        <v>202</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4047,10 +4049,10 @@
         <v>12</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>31</v>
@@ -4059,10 +4061,10 @@
         <v>8</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="R115" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="116" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4073,10 +4075,10 @@
         <v>12</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>31</v>
@@ -4085,10 +4087,10 @@
         <v>8</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>83</v>
+        <v>200</v>
       </c>
       <c r="R116" s="3" t="s">
-        <v>118</v>
+        <v>199</v>
       </c>
     </row>
     <row r="117" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4099,10 +4101,10 @@
         <v>12</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>31</v>
@@ -4111,10 +4113,10 @@
         <v>8</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R117" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="118" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4125,10 +4127,10 @@
         <v>12</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>31</v>
@@ -4137,10 +4139,10 @@
         <v>8</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="R118" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="119" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4151,10 +4153,10 @@
         <v>12</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>31</v>
@@ -4163,10 +4165,10 @@
         <v>8</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="R119" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="120" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4177,10 +4179,10 @@
         <v>12</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>31</v>
@@ -4189,10 +4191,10 @@
         <v>8</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="R120" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="121" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4203,10 +4205,10 @@
         <v>12</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>31</v>
@@ -4215,10 +4217,10 @@
         <v>8</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="R121" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="122" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4229,10 +4231,10 @@
         <v>12</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>31</v>
@@ -4241,10 +4243,10 @@
         <v>8</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R122" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4255,10 +4257,10 @@
         <v>12</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>31</v>
@@ -4267,10 +4269,10 @@
         <v>8</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="R123" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4281,10 +4283,10 @@
         <v>12</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>31</v>
@@ -4293,10 +4295,10 @@
         <v>8</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>145</v>
+        <v>42</v>
       </c>
       <c r="R124" s="3" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4307,10 +4309,10 @@
         <v>12</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>31</v>
@@ -4319,10 +4321,10 @@
         <v>8</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="R125" s="3" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
     <row r="126" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4333,10 +4335,10 @@
         <v>12</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>31</v>
@@ -4345,10 +4347,10 @@
         <v>8</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="R126" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4359,10 +4361,10 @@
         <v>12</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>31</v>
@@ -4371,10 +4373,10 @@
         <v>8</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="R127" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4385,10 +4387,10 @@
         <v>12</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>31</v>
@@ -4397,10 +4399,10 @@
         <v>8</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="R128" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4411,10 +4413,10 @@
         <v>12</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>31</v>
@@ -4423,10 +4425,10 @@
         <v>8</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="R129" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4437,10 +4439,10 @@
         <v>12</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>31</v>
@@ -4449,10 +4451,10 @@
         <v>8</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="R130" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4463,10 +4465,10 @@
         <v>12</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>31</v>
@@ -4475,10 +4477,10 @@
         <v>8</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="R131" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4489,10 +4491,10 @@
         <v>12</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>31</v>
@@ -4501,10 +4503,10 @@
         <v>8</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R132" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4515,10 +4517,10 @@
         <v>12</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>31</v>
@@ -4527,10 +4529,10 @@
         <v>8</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R133" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4541,10 +4543,10 @@
         <v>12</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>31</v>
@@ -4553,10 +4555,10 @@
         <v>8</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="R134" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4567,10 +4569,10 @@
         <v>12</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>31</v>
@@ -4579,10 +4581,10 @@
         <v>8</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>261</v>
+        <v>44</v>
       </c>
       <c r="R135" s="3" t="s">
-        <v>262</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4593,10 +4595,10 @@
         <v>12</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>31</v>
@@ -4605,10 +4607,10 @@
         <v>8</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>93</v>
+        <v>261</v>
       </c>
       <c r="R136" s="3" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
     </row>
     <row r="137" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4619,10 +4621,10 @@
         <v>12</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>31</v>
@@ -4631,10 +4633,10 @@
         <v>8</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>204</v>
+        <v>93</v>
       </c>
       <c r="R137" s="3" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -4645,7 +4647,7 @@
         <v>12</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>256</v>
@@ -4657,30 +4659,36 @@
         <v>8</v>
       </c>
       <c r="I138" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="R138" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I139" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="R138" s="3" t="s">
+      <c r="R139" s="3" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D139" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E139" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G139" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="140" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -4691,10 +4699,10 @@
         <v>12</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>36</v>
@@ -4711,10 +4719,10 @@
         <v>12</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E141" s="4" t="s">
         <v>36</v>
@@ -4731,10 +4739,10 @@
         <v>12</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E142" s="4" t="s">
         <v>36</v>
@@ -4751,13 +4759,13 @@
         <v>12</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G143" s="4" t="s">
         <v>8</v>
@@ -4771,10 +4779,10 @@
         <v>12</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E144" s="4" t="s">
         <v>37</v>
@@ -4791,10 +4799,10 @@
         <v>12</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E145" s="4" t="s">
         <v>37</v>
@@ -4811,10 +4819,10 @@
         <v>12</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E146" s="4" t="s">
         <v>37</v>
@@ -4823,15 +4831,35 @@
         <v>8</v>
       </c>
     </row>
+    <row r="147" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G147" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:T146" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T147" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="J1:P1048576">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(OR($B1="O365Group",$B1="Type"),faslch,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="T20" r:id="rId1" xr:uid="{6406F3B4-332F-49FC-A4BF-E9A46FEED504}"/>
+    <hyperlink ref="T21" r:id="rId1" xr:uid="{6406F3B4-332F-49FC-A4BF-E9A46FEED504}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4839,6 +4867,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -5022,35 +5065,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5072,9 +5090,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sync with public repo and group updates
</commit_message>
<xml_diff>
--- a/data/aad/Gruppen-Basic-ADSync.xlsx
+++ b/data/aad/Gruppen-Basic-ADSync.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38025EA3-AE86-4AD8-924B-0FE764F8B72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C223D6B4-A03E-40C3-AE94-C37FA833A6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="30804" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="30960" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gruppen!$A$1:$T$147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gruppen!$A$1:$T$189</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="338">
   <si>
     <t>Type</t>
   </si>
@@ -874,6 +874,174 @@
   </si>
   <si>
     <t>Legacy Auth is not blocked by conditional Access for members in this group</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365BCP</t>
+  </si>
+  <si>
+    <t>DYN365_BUSCENTRAL_PREMIUM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365SALES</t>
+  </si>
+  <si>
+    <t>DYN365_ENTERPRISE_SALES</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365TEAM</t>
+  </si>
+  <si>
+    <t>DYN365_TEAM_MEMBERS</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-EXCHP2</t>
+  </si>
+  <si>
+    <t>EXCHANGEENTERPRISE</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-OFFICEAPPS</t>
+  </si>
+  <si>
+    <t>OFFICESUBSCRIPTION</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-TEAMSPREM</t>
+  </si>
+  <si>
+    <t>Microsoft_Teams_Premium</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-MS365BUSAPPS</t>
+  </si>
+  <si>
+    <t>O365_BUSINESS</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PBIPREM</t>
+  </si>
+  <si>
+    <t>PBI_PREMIUM_PER_USER</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PAPPSPREM</t>
+  </si>
+  <si>
+    <t>POWERAPPS_PER_USER</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PAUTOPREM</t>
+  </si>
+  <si>
+    <t>POWERAUTOMATE_ATTENDED_RPA</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PROJECT5</t>
+  </si>
+  <si>
+    <t>PROJECTPREMIUM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-A3LEHR</t>
+  </si>
+  <si>
+    <t>M365EDU_A3_FACULTY</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-A3STUD</t>
+  </si>
+  <si>
+    <t>M365EDU_A3_STUUSEBNFT</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-RMADHOC</t>
+  </si>
+  <si>
+    <t>RIGHTSMANAGEMENT_ADHOC</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365BCPONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365SALESONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365TEAMONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-EXCHP2ONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-OFFICEAPPSONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-TEAMSPREMONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-MS365BUSAPPSONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PBIPREMONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PAPPSPREMONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PAUTOPREMONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PROJECT5ONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-A3LEHRONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-A3STUDONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-RMADHOCONPREM</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365BCPCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365SALESCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-DYN365TEAMCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-EXCHP2CLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-OFFICEAPPSCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-TEAMSPREMCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-MS365BUSAPPSCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PBIPREMCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PAPPSPREMCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PAUTOPREMCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-PROJECT5CLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-A3LEHRCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-A3STUDCLOUD</t>
+  </si>
+  <si>
+    <t>ALYASG-LIC-RMADHOCCLOUD</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T147"/>
+  <dimension ref="A1:T189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -2502,7 +2670,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>23</v>
       </c>
@@ -2525,7 +2693,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>23</v>
       </c>
@@ -2548,7 +2716,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>23</v>
       </c>
@@ -2571,7 +2739,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
@@ -2594,7 +2762,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>23</v>
       </c>
@@ -2617,7 +2785,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2640,7 +2808,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="55" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>23</v>
       </c>
@@ -2663,7 +2831,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="56" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>23</v>
       </c>
@@ -2683,7 +2851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>23</v>
       </c>
@@ -2703,7 +2871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>23</v>
       </c>
@@ -2723,7 +2891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>23</v>
       </c>
@@ -2743,7 +2911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>23</v>
       </c>
@@ -2763,7 +2931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>23</v>
       </c>
@@ -2783,7 +2951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>23</v>
       </c>
@@ -2791,10 +2959,10 @@
         <v>12</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>31</v>
@@ -2802,11 +2970,11 @@
       <c r="G62" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R62" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I62" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>23</v>
       </c>
@@ -2814,10 +2982,10 @@
         <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>120</v>
+        <v>284</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>120</v>
+        <v>284</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>31</v>
@@ -2825,8 +2993,11 @@
       <c r="G63" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I63" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>23</v>
       </c>
@@ -2834,16 +3005,19 @@
         <v>12</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>121</v>
+        <v>286</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>121</v>
+        <v>286</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="65" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2854,16 +3028,19 @@
         <v>12</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="R65" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2874,10 +3051,10 @@
         <v>12</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>31</v>
@@ -2894,10 +3071,10 @@
         <v>12</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>31</v>
@@ -2914,16 +3091,19 @@
         <v>12</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>125</v>
+        <v>288</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>125</v>
+        <v>288</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="69" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2934,19 +3114,16 @@
         <v>12</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="R69" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2957,19 +3134,16 @@
         <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="R70" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2980,10 +3154,10 @@
         <v>12</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>127</v>
+        <v>290</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>127</v>
+        <v>290</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>31</v>
@@ -2991,8 +3165,8 @@
       <c r="G71" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R71" s="3" t="s">
-        <v>160</v>
+      <c r="I71" s="3" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="72" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3003,10 +3177,10 @@
         <v>12</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>31</v>
@@ -3023,10 +3197,10 @@
         <v>12</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>31</v>
@@ -3043,16 +3217,19 @@
         <v>12</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="R74" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3063,16 +3240,19 @@
         <v>12</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>131</v>
+        <v>292</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>131</v>
+        <v>292</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="76" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3083,16 +3263,19 @@
         <v>12</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>132</v>
+        <v>294</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>132</v>
+        <v>294</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3103,16 +3286,19 @@
         <v>12</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="R77" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3123,16 +3309,19 @@
         <v>12</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3143,10 +3332,10 @@
         <v>12</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>31</v>
@@ -3163,10 +3352,10 @@
         <v>12</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>262</v>
+        <v>129</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>262</v>
+        <v>129</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>31</v>
@@ -3183,10 +3372,10 @@
         <v>12</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>31</v>
@@ -3203,10 +3392,10 @@
         <v>12</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>203</v>
+        <v>131</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>203</v>
+        <v>131</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>31</v>
@@ -3223,380 +3412,323 @@
         <v>12</v>
       </c>
       <c r="C83" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D94" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E83" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I84" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="R84" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I85" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="R85" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G86" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I86" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="R86" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I87" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="R87" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I88" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="R88" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I89" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="R89" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G90" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I90" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="R90" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G91" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I91" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R91" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I92" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="R92" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G93" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I93" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R93" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G94" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I94" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R94" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G95" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I95" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="R95" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G96" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I96" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="R96" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G97" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I97" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="R97" s="6" t="s">
-        <v>146</v>
+      <c r="E94" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="R95" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="R96" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="98" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3607,10 +3739,10 @@
         <v>190</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>31</v>
@@ -3619,10 +3751,10 @@
         <v>8</v>
       </c>
       <c r="I98" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="R98" s="6" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3633,10 +3765,10 @@
         <v>190</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>31</v>
@@ -3645,10 +3777,10 @@
         <v>8</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>43</v>
+        <v>159</v>
       </c>
       <c r="R99" s="6" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
     </row>
     <row r="100" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3659,10 +3791,10 @@
         <v>190</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>31</v>
@@ -3671,10 +3803,10 @@
         <v>8</v>
       </c>
       <c r="I100" s="6" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="R100" s="6" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3685,10 +3817,10 @@
         <v>190</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>31</v>
@@ -3697,10 +3829,10 @@
         <v>8</v>
       </c>
       <c r="I101" s="6" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="R101" s="6" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3711,10 +3843,10 @@
         <v>190</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>31</v>
@@ -3723,10 +3855,10 @@
         <v>8</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>34</v>
+        <v>200</v>
       </c>
       <c r="R102" s="6" t="s">
-        <v>130</v>
+        <v>199</v>
       </c>
     </row>
     <row r="103" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3737,10 +3869,10 @@
         <v>190</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>31</v>
@@ -3749,10 +3881,10 @@
         <v>8</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="R103" s="6" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3763,10 +3895,10 @@
         <v>190</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>225</v>
+        <v>310</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>225</v>
+        <v>310</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>31</v>
@@ -3775,10 +3907,10 @@
         <v>8</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>90</v>
+        <v>283</v>
       </c>
       <c r="R104" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
     </row>
     <row r="105" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3789,10 +3921,10 @@
         <v>190</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>227</v>
+        <v>311</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>227</v>
+        <v>311</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>31</v>
@@ -3801,10 +3933,10 @@
         <v>8</v>
       </c>
       <c r="I105" s="6" t="s">
-        <v>91</v>
+        <v>285</v>
       </c>
       <c r="R105" s="6" t="s">
-        <v>133</v>
+        <v>284</v>
       </c>
     </row>
     <row r="106" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3815,10 +3947,10 @@
         <v>190</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>226</v>
+        <v>312</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>226</v>
+        <v>312</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>31</v>
@@ -3827,10 +3959,10 @@
         <v>8</v>
       </c>
       <c r="I106" s="6" t="s">
-        <v>92</v>
+        <v>287</v>
       </c>
       <c r="R106" s="6" t="s">
-        <v>134</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3841,10 +3973,10 @@
         <v>190</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="E107" s="6" t="s">
         <v>31</v>
@@ -3853,10 +3985,10 @@
         <v>8</v>
       </c>
       <c r="I107" s="6" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="R107" s="6" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3867,10 +3999,10 @@
         <v>190</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>266</v>
+        <v>212</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>266</v>
+        <v>212</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>31</v>
@@ -3879,10 +4011,10 @@
         <v>8</v>
       </c>
       <c r="I108" s="6" t="s">
-        <v>261</v>
+        <v>33</v>
       </c>
       <c r="R108" s="6" t="s">
-        <v>262</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3893,10 +4025,10 @@
         <v>190</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>31</v>
@@ -3905,10 +4037,10 @@
         <v>8</v>
       </c>
       <c r="I109" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="R109" s="6" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3919,10 +4051,10 @@
         <v>190</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>230</v>
+        <v>313</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>230</v>
+        <v>313</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>31</v>
@@ -3931,10 +4063,10 @@
         <v>8</v>
       </c>
       <c r="I110" s="6" t="s">
-        <v>204</v>
+        <v>289</v>
       </c>
       <c r="R110" s="6" t="s">
-        <v>203</v>
+        <v>288</v>
       </c>
     </row>
     <row r="111" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3945,914 +4077,2006 @@
         <v>190</v>
       </c>
       <c r="C111" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I111" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R111" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I112" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="R112" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G113" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I113" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="R113" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G114" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I114" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R114" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G115" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I115" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R115" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I116" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="R116" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I117" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="R117" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="R118" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I119" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="R119" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G120" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I120" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="R120" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I121" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R121" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G122" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I122" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="R122" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G123" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I123" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R123" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G124" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I124" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R124" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G125" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="R125" s="6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G126" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I126" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="R126" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G127" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I127" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="R127" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G128" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I128" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="R128" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G129" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I129" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="R129" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I130" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="R130" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G131" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I131" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R131" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G132" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I132" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="R132" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G133" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I133" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="R133" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G134" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I134" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="R134" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G135" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I135" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="R135" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C136" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="D111" s="6" t="s">
+      <c r="D136" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="E111" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G111" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I111" s="6" t="s">
+      <c r="E136" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G136" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I136" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="R111" s="6" t="s">
+      <c r="R136" s="6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="112" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C112" s="3" t="s">
+    <row r="137" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G137" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I137" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="R137" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E138" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G138" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I138" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="R138" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G139" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I139" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="R139" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C140" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D140" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="E112" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I112" s="3" t="s">
+      <c r="E140" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I140" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="R112" s="3" t="s">
+      <c r="R140" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="113" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C113" s="3" t="s">
+    <row r="141" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D141" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E113" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I113" s="3" t="s">
+      <c r="E141" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I141" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="R113" s="3" t="s">
+      <c r="R141" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="114" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C114" s="3" t="s">
+    <row r="142" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D142" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E114" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I114" s="3" t="s">
+      <c r="E142" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I142" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="R114" s="3" t="s">
+      <c r="R142" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C115" s="3" t="s">
+    <row r="143" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D143" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="E115" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G115" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I115" s="3" t="s">
+      <c r="E143" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I143" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="R115" s="3" t="s">
+      <c r="R143" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="116" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C116" s="3" t="s">
+    <row r="144" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D144" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E116" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I116" s="3" t="s">
+      <c r="E144" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I144" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="R116" s="3" t="s">
+      <c r="R144" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="117" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C117" s="3" t="s">
+    <row r="145" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D145" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E117" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I117" s="3" t="s">
+      <c r="E145" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I145" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="R117" s="3" t="s">
+      <c r="R145" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="118" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C118" s="3" t="s">
+    <row r="146" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="R146" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="R147" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="R148" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D149" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E118" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G118" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I118" s="3" t="s">
+      <c r="E149" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I149" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="R118" s="3" t="s">
+      <c r="R149" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="119" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C119" s="3" t="s">
+    <row r="150" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D150" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="E119" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I119" s="3" t="s">
+      <c r="E150" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I150" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R119" s="3" t="s">
+      <c r="R150" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C120" s="3" t="s">
+    <row r="151" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C151" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D120" s="3" t="s">
+      <c r="D151" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="E120" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I120" s="3" t="s">
+      <c r="E151" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I151" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="R120" s="3" t="s">
+      <c r="R151" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="121" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C121" s="3" t="s">
+    <row r="152" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="R152" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C153" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D153" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="E121" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G121" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I121" s="3" t="s">
+      <c r="E153" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I153" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R121" s="3" t="s">
+      <c r="R153" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="122" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C122" s="3" t="s">
+    <row r="154" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C154" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D122" s="3" t="s">
+      <c r="D154" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="E122" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I122" s="3" t="s">
+      <c r="E154" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I154" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="R122" s="3" t="s">
+      <c r="R154" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="123" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C123" s="3" t="s">
+    <row r="155" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="R155" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C156" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D156" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="E123" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G123" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I123" s="3" t="s">
+      <c r="E156" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I156" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="R123" s="3" t="s">
+      <c r="R156" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="124" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C124" s="3" t="s">
+    <row r="157" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D157" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E124" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I124" s="3" t="s">
+      <c r="E157" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I157" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="R124" s="3" t="s">
+      <c r="R157" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="125" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C125" s="3" t="s">
+    <row r="158" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C158" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D125" s="3" t="s">
+      <c r="D158" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E125" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G125" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I125" s="3" t="s">
+      <c r="E158" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I158" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="R125" s="3" t="s">
+      <c r="R158" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="3" t="s">
+    <row r="159" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G159" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="R159" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I160" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="R160" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D126" s="3" t="s">
+      <c r="D161" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E126" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I126" s="3" t="s">
+      <c r="E161" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G161" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I161" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="R126" s="3" t="s">
+      <c r="R161" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C127" s="3" t="s">
+    <row r="162" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D162" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E127" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G127" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I127" s="3" t="s">
+      <c r="E162" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G162" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I162" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="R127" s="3" t="s">
+      <c r="R162" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C128" s="3" t="s">
+    <row r="163" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C163" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="D163" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="E128" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I128" s="3" t="s">
+      <c r="E163" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G163" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I163" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="R128" s="3" t="s">
+      <c r="R163" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C129" s="3" t="s">
+    <row r="164" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C164" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D129" s="3" t="s">
+      <c r="D164" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E129" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I129" s="3" t="s">
+      <c r="E164" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I164" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="R129" s="3" t="s">
+      <c r="R164" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C130" s="3" t="s">
+    <row r="165" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C165" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D165" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="E130" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G130" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I130" s="3" t="s">
+      <c r="E165" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I165" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="R130" s="3" t="s">
+      <c r="R165" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="131" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C131" s="3" t="s">
+    <row r="166" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D131" s="3" t="s">
+      <c r="D166" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="E131" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G131" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I131" s="3" t="s">
+      <c r="E166" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I166" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="R131" s="3" t="s">
+      <c r="R166" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C132" s="3" t="s">
+    <row r="167" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I167" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="R167" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I168" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="R168" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I169" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="R169" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C170" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D132" s="3" t="s">
+      <c r="D170" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E132" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G132" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I132" s="3" t="s">
+      <c r="E170" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I170" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R132" s="3" t="s">
+      <c r="R170" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="133" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C133" s="3" t="s">
+    <row r="171" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C171" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D133" s="3" t="s">
+      <c r="D171" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E133" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G133" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I133" s="3" t="s">
+      <c r="E171" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I171" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="R133" s="3" t="s">
+      <c r="R171" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C134" s="3" t="s">
+    <row r="172" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C172" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D172" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E134" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G134" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I134" s="3" t="s">
+      <c r="E172" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I172" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="R134" s="3" t="s">
+      <c r="R172" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C135" s="3" t="s">
+    <row r="173" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C173" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D135" s="3" t="s">
+      <c r="D173" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E135" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G135" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I135" s="3" t="s">
+      <c r="E173" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I173" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R135" s="3" t="s">
+      <c r="R173" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C136" s="3" t="s">
+    <row r="174" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C174" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D136" s="3" t="s">
+      <c r="D174" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="E136" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I136" s="3" t="s">
+      <c r="E174" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I174" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="R136" s="3" t="s">
+      <c r="R174" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="137" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C137" s="3" t="s">
+    <row r="175" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I175" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="R175" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C176" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="D176" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="E137" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G137" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I137" s="3" t="s">
+      <c r="E176" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I176" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="R137" s="3" t="s">
+      <c r="R176" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C138" s="3" t="s">
+    <row r="177" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C177" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D138" s="3" t="s">
+      <c r="D177" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E138" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I138" s="3" t="s">
+      <c r="E177" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I177" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="R138" s="3" t="s">
+      <c r="R177" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="139" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C139" s="3" t="s">
+    <row r="178" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C178" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="D139" s="3" t="s">
+      <c r="D178" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E139" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G139" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I139" s="3" t="s">
+      <c r="E178" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I178" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="R139" s="3" t="s">
+      <c r="R178" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="140" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C140" s="4" t="s">
+    <row r="179" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I179" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="R179" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I180" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="R180" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I181" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="R181" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C182" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D140" s="4" t="s">
+      <c r="D182" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E140" s="4" t="s">
+      <c r="E182" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G140" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C141" s="4" t="s">
+      <c r="G182" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C183" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D183" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E141" s="4" t="s">
+      <c r="E183" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G141" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C142" s="4" t="s">
+      <c r="G183" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C184" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="D184" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E142" s="4" t="s">
+      <c r="E184" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G142" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C143" s="4" t="s">
+      <c r="G184" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C185" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D185" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E143" s="4" t="s">
+      <c r="E185" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G143" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C144" s="4" t="s">
+      <c r="G185" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C186" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D144" s="4" t="s">
+      <c r="D186" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E144" s="4" t="s">
+      <c r="E186" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G144" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C145" s="4" t="s">
+      <c r="G186" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C187" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D145" s="4" t="s">
+      <c r="D187" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E145" s="4" t="s">
+      <c r="E187" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G145" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C146" s="4" t="s">
+      <c r="G187" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C188" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="D188" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E146" s="4" t="s">
+      <c r="E188" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G146" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C147" s="4" t="s">
+      <c r="G188" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C189" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D147" s="4" t="s">
+      <c r="D189" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E147" s="4" t="s">
+      <c r="E189" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G147" s="4" t="s">
+      <c r="G189" s="4" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T147" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T189" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="J1:P1048576">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(OR($B1="O365Group",$B1="Type"),faslch,TRUE)</formula>
@@ -4867,21 +6091,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -5065,10 +6274,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5090,19 +6324,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2534DDDA-BE8A-43DA-A0C1-B6D96DC767B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB80E815-258B-4085-B06C-0327483055A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>